<commit_message>
5/12 end of lab uplaod
</commit_message>
<xml_diff>
--- a/Docs/v_line/v_line_memory_map.xlsx
+++ b/Docs/v_line/v_line_memory_map.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="48">
+  <si>
+    <t/>
+  </si>
   <si>
     <t>C1</t>
   </si>
@@ -162,7 +165,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +176,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -190,7 +199,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -217,18 +233,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -547,409 +566,411 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="3.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="3.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="K6" s="5"/>
       <c r="L6" s="3"/>
       <c r="M6" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R6" s="3"/>
       <c r="S6" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>

</xml_diff>